<commit_message>
Modified spreadsheet to include auto-highlighting
Modified focal length scale and set up conditional formatting to automatically highlight focal length range
</commit_message>
<xml_diff>
--- a/LensInventory.xlsx
+++ b/LensInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\cust\photo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaletz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F67AEE2-5F1C-47D2-A365-0AA3717DDB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B763C57-ACC3-499D-83C5-2648D5AA8C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{92D27A56-3DF6-4B0D-8D53-B909E89173A1}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{92D27A56-3DF6-4B0D-8D53-B909E89173A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,11 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$6:$B$12</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$5</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$6:$D$12</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$E$5</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$E$6:$E$12</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$6:$C$12</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$5</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$6:$D$12</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$5</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$E$6:$E$12</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$6:$B$12</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$6:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>Vendor</t>
   </si>
@@ -254,6 +247,26 @@
   </si>
   <si>
     <t>Modern / AF (KP / Current Kit)</t>
+  </si>
+  <si>
+    <t>MIN 
+FOCAL LENGTH</t>
+  </si>
+  <si>
+    <t>MAX 
+FOCAL LENGTH</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>Prime</t>
+  </si>
+  <si>
+    <t>LENS TYPE</t>
+  </si>
+  <si>
+    <t>Pentax 11-18</t>
   </si>
 </sst>
 </file>
@@ -299,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,21 +321,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -331,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -340,8 +358,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -350,9 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -375,15 +388,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -401,26 +445,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -431,7 +475,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{17A66C12-E362-47D5-B26B-1321CE130B8A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>L</cx:v>
             </cx:txData>
           </cx:tx>
@@ -444,7 +488,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4C4C4B11-3195-47E0-8DA3-5427725CCFCE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>P</cx:v>
             </cx:txData>
           </cx:tx>
@@ -457,7 +501,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{21A375DC-4938-4134-B6A4-DA141C4D3BBA}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>H</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1086,8 +1130,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5774055" y="899160"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="5476875" y="929640"/>
+              <a:ext cx="4358640" cy="2857500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1409,7 +1453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1423,12 +1467,12 @@
       <selection activeCell="C70" sqref="C70:AB70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5234375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1453,7 +1497,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1508,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1475,7 +1519,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1486,7 +1530,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1494,7 +1538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1502,7 +1546,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1554,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
@@ -1553,7 +1597,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1611,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1584,161 +1628,161 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F44">
         <f>F43+25</f>
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F45">
-        <f t="shared" ref="F45:F100" si="0">F44+25</f>
+        <f t="shared" ref="F45:F67" si="0">F44+25</f>
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F46">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F47">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F48">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54">
         <f t="shared" si="0"/>
         <v>275</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56">
         <f t="shared" si="0"/>
         <v>325</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58">
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F62">
         <f t="shared" si="0"/>
         <v>475</v>
       </c>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F63">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F64">
         <f t="shared" si="0"/>
         <v>525</v>
       </c>
     </row>
-    <row r="65" spans="3:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="3:28" x14ac:dyDescent="0.25">
       <c r="F65">
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
     </row>
-    <row r="66" spans="3:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="3:28" x14ac:dyDescent="0.25">
       <c r="F66">
         <f t="shared" si="0"/>
         <v>575</v>
       </c>
     </row>
-    <row r="67" spans="3:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="3:28" x14ac:dyDescent="0.25">
       <c r="F67">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
-    <row r="70" spans="3:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>11</v>
       </c>
@@ -1746,99 +1790,99 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <f>D70+25</f>
+        <f t="shared" ref="E70:AB70" si="1">D70+25</f>
         <v>25</v>
       </c>
       <c r="F70">
-        <f>E70+25</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="G70">
-        <f>F70+25</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="H70">
-        <f>G70+25</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="I70">
-        <f>H70+25</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="J70">
-        <f>I70+25</f>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="K70">
-        <f>J70+25</f>
+        <f t="shared" si="1"/>
         <v>175</v>
       </c>
       <c r="L70">
-        <f>K70+25</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="M70">
-        <f>L70+25</f>
+        <f t="shared" si="1"/>
         <v>225</v>
       </c>
       <c r="N70">
-        <f>M70+25</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="O70">
-        <f>N70+25</f>
+        <f t="shared" si="1"/>
         <v>275</v>
       </c>
       <c r="P70">
-        <f>O70+25</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="Q70">
-        <f>P70+25</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="R70">
-        <f>Q70+25</f>
+        <f t="shared" si="1"/>
         <v>350</v>
       </c>
       <c r="S70">
-        <f>R70+25</f>
+        <f t="shared" si="1"/>
         <v>375</v>
       </c>
       <c r="T70">
-        <f>S70+25</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="U70">
-        <f>T70+25</f>
+        <f t="shared" si="1"/>
         <v>425</v>
       </c>
       <c r="V70">
-        <f>U70+25</f>
+        <f t="shared" si="1"/>
         <v>450</v>
       </c>
       <c r="W70">
-        <f>V70+25</f>
+        <f t="shared" si="1"/>
         <v>475</v>
       </c>
       <c r="X70">
-        <f>W70+25</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="Y70">
-        <f>X70+25</f>
+        <f t="shared" si="1"/>
         <v>525</v>
       </c>
       <c r="Z70">
-        <f>Y70+25</f>
+        <f t="shared" si="1"/>
         <v>550</v>
       </c>
       <c r="AA70">
-        <f>Z70+25</f>
+        <f t="shared" si="1"/>
         <v>575</v>
       </c>
       <c r="AB70">
-        <f>AA70+25</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -1851,801 +1895,2483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CDC258-A19D-40F0-932A-28A5C117CBBA}">
-  <dimension ref="A1:BN32"/>
+  <dimension ref="A1:CE32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.20703125" customWidth="1"/>
-    <col min="3" max="3" width="10.15625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3671875" style="11" customWidth="1"/>
-    <col min="6" max="66" width="2.1015625" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="8" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" style="8" hidden="1" customWidth="1"/>
+    <col min="9" max="70" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="15" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:83" s="12" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17"/>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-      <c r="BB1" s="17"/>
-      <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="14"/>
+      <c r="BJ1" s="14"/>
+      <c r="BK1" s="14"/>
+      <c r="BL1" s="14"/>
+      <c r="BM1" s="14"/>
+      <c r="BN1" s="14"/>
+      <c r="BO1" s="14"/>
+      <c r="BP1" s="14"/>
+      <c r="BQ1" s="14"/>
+      <c r="BR1" s="14"/>
+    </row>
+    <row r="2" spans="1:83" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="17"/>
+      <c r="E2" s="9"/>
+      <c r="I2" s="21">
+        <v>0</v>
+      </c>
+      <c r="J2" s="21">
+        <v>10</v>
+      </c>
+      <c r="K2" s="21">
+        <f>J2+2</f>
+        <v>12</v>
+      </c>
+      <c r="L2" s="21">
+        <f t="shared" ref="L2:Q2" si="0">K2+2</f>
+        <v>14</v>
+      </c>
+      <c r="M2" s="21">
+        <v>15</v>
+      </c>
+      <c r="N2" s="21">
+        <v>18</v>
+      </c>
+      <c r="O2" s="21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P2" s="21">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="Q2" s="22">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="R2" s="21">
+        <f>Q2+4</f>
+        <v>28</v>
+      </c>
+      <c r="S2" s="21">
+        <v>30</v>
+      </c>
+      <c r="T2" s="21">
+        <f t="shared" ref="T2:Y2" si="1">S2+5</f>
+        <v>35</v>
+      </c>
+      <c r="U2" s="21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="V2" s="21">
+        <v>43</v>
+      </c>
+      <c r="W2" s="22">
+        <v>50</v>
+      </c>
+      <c r="X2" s="21">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="Y2" s="21">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="Z2" s="21">
+        <v>70</v>
+      </c>
+      <c r="AA2" s="21">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="21">
+        <v>80</v>
+      </c>
+      <c r="AC2" s="21">
+        <v>85</v>
+      </c>
+      <c r="AD2" s="21">
+        <f>AB2+10</f>
+        <v>90</v>
+      </c>
+      <c r="AE2" s="22">
+        <f t="shared" ref="AE2:AM2" si="2">AD2+10</f>
+        <v>100</v>
+      </c>
+      <c r="AF2" s="21">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="AG2" s="21">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="AH2" s="21">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="AI2" s="21">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="AJ2" s="21">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="AK2" s="21">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="AL2" s="21">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="AM2" s="21">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="AN2" s="22">
+        <f>AM2+20</f>
+        <v>200</v>
+      </c>
+      <c r="AO2" s="21">
+        <f t="shared" ref="AO2:BR2" si="3">AN2+20</f>
+        <v>220</v>
+      </c>
+      <c r="AP2" s="21">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="AQ2" s="21">
+        <f t="shared" si="3"/>
+        <v>260</v>
+      </c>
+      <c r="AR2" s="21">
+        <f t="shared" si="3"/>
+        <v>280</v>
+      </c>
+      <c r="AS2" s="22">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="AT2" s="21">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+      <c r="AU2" s="21">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+      <c r="AV2" s="21">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="AW2" s="21">
+        <f t="shared" si="3"/>
+        <v>380</v>
+      </c>
+      <c r="AX2" s="22">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="AY2" s="21">
+        <f t="shared" si="3"/>
+        <v>420</v>
+      </c>
+      <c r="AZ2" s="21">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+      <c r="BA2" s="21">
+        <f t="shared" si="3"/>
+        <v>460</v>
+      </c>
+      <c r="BB2" s="21">
+        <f t="shared" si="3"/>
+        <v>480</v>
+      </c>
+      <c r="BC2" s="22">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="BD2" s="21">
+        <f>BC2+20</f>
+        <v>520</v>
+      </c>
+      <c r="BE2" s="21">
+        <f t="shared" si="3"/>
+        <v>540</v>
+      </c>
+      <c r="BF2" s="21">
+        <f t="shared" si="3"/>
+        <v>560</v>
+      </c>
+      <c r="BG2" s="21">
+        <f t="shared" si="3"/>
+        <v>580</v>
+      </c>
+      <c r="BH2" s="22">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="BI2" s="21">
+        <f>BH2+20</f>
+        <v>620</v>
+      </c>
+      <c r="BJ2" s="21">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+      <c r="BK2" s="21">
+        <f t="shared" si="3"/>
+        <v>660</v>
+      </c>
+      <c r="BL2" s="21">
+        <f t="shared" si="3"/>
+        <v>680</v>
+      </c>
+      <c r="BM2" s="22">
+        <f t="shared" si="3"/>
+        <v>700</v>
+      </c>
+      <c r="BN2" s="21">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="BO2" s="21">
+        <f t="shared" si="3"/>
+        <v>740</v>
+      </c>
+      <c r="BP2" s="21">
+        <f t="shared" si="3"/>
+        <v>760</v>
+      </c>
+      <c r="BQ2" s="21">
+        <f t="shared" si="3"/>
+        <v>780</v>
+      </c>
+      <c r="BR2" s="22">
+        <f t="shared" si="3"/>
+        <v>800</v>
+      </c>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+    </row>
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="8">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8">
+        <f>IF(C3="Zoom",VALUE(RIGHT(D3,LEN(D3)-FIND("-",D3))),D3)</f>
+        <v>135</v>
+      </c>
+      <c r="Q3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BR3" s="23"/>
+    </row>
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="18">
         <v>100</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="8">
+        <v>100</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" ref="H4:H8" si="4">IF(C4="Zoom",VALUE(RIGHT(D4,LEN(D4)-FIND("-",D4))),D4)</f>
+        <v>100</v>
+      </c>
+      <c r="Q4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BH4" s="23"/>
+      <c r="BM4" s="23"/>
+      <c r="BR4" s="23"/>
+    </row>
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="8">
+        <v>55</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="24"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="24"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="24"/>
+      <c r="AY5" s="15"/>
+      <c r="AZ5" s="15"/>
+      <c r="BA5" s="15"/>
+      <c r="BB5" s="15"/>
+      <c r="BC5" s="24"/>
+      <c r="BD5" s="15"/>
+      <c r="BE5" s="15"/>
+      <c r="BF5" s="15"/>
+      <c r="BG5" s="15"/>
+      <c r="BH5" s="24"/>
+      <c r="BI5" s="15"/>
+      <c r="BJ5" s="15"/>
+      <c r="BK5" s="15"/>
+      <c r="BL5" s="15"/>
+      <c r="BM5" s="24"/>
+      <c r="BN5" s="15"/>
+      <c r="BO5" s="15"/>
+      <c r="BP5" s="15"/>
+      <c r="BR5" s="24"/>
+    </row>
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="4"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
-      <c r="AY6" s="4"/>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="8">
+        <v>150</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="4"/>
+        <v>450</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="24"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="24"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="24"/>
+      <c r="AY6" s="15"/>
+      <c r="AZ6" s="15"/>
+      <c r="BA6" s="15"/>
+      <c r="BB6" s="15"/>
+      <c r="BC6" s="24"/>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="15"/>
+      <c r="BF6" s="15"/>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="24"/>
+      <c r="BI6" s="15"/>
+      <c r="BJ6" s="15"/>
+      <c r="BK6" s="15"/>
+      <c r="BL6" s="15"/>
+      <c r="BM6" s="24"/>
+      <c r="BN6" s="15"/>
+      <c r="BO6" s="15"/>
+      <c r="BP6" s="15"/>
+      <c r="BR6" s="24"/>
+    </row>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="str">
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="18" t="str">
         <f>"10-20"</f>
         <v>10-20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.55000000000000004">
-      <c r="D8" s="11"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="10">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="15"/>
+      <c r="AN7" s="24"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="15"/>
+      <c r="AQ7" s="15"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="24"/>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="24"/>
+      <c r="AY7" s="15"/>
+      <c r="AZ7" s="15"/>
+      <c r="BA7" s="15"/>
+      <c r="BB7" s="15"/>
+      <c r="BC7" s="24"/>
+      <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
+      <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="24"/>
+      <c r="BI7" s="15"/>
+      <c r="BJ7" s="15"/>
+      <c r="BK7" s="15"/>
+      <c r="BL7" s="15"/>
+      <c r="BM7" s="24"/>
+      <c r="BN7" s="15"/>
+      <c r="BO7" s="15"/>
+      <c r="BP7" s="15"/>
+      <c r="BR7" s="24"/>
+    </row>
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="20" t="str">
+        <f>"11-18"</f>
+        <v>11-18</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="10">
+        <v>10</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="15"/>
+      <c r="AJ8" s="15"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
+      <c r="AN8" s="24"/>
+      <c r="AO8" s="15"/>
+      <c r="AP8" s="15"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
+      <c r="AS8" s="24"/>
+      <c r="AT8" s="15"/>
+      <c r="AU8" s="15"/>
+      <c r="AV8" s="15"/>
+      <c r="AW8" s="15"/>
+      <c r="AX8" s="24"/>
+      <c r="AY8" s="15"/>
+      <c r="AZ8" s="15"/>
+      <c r="BA8" s="15"/>
+      <c r="BB8" s="15"/>
+      <c r="BC8" s="24"/>
+      <c r="BD8" s="15"/>
+      <c r="BE8" s="15"/>
+      <c r="BF8" s="15"/>
+      <c r="BG8" s="15"/>
+      <c r="BH8" s="24"/>
+      <c r="BI8" s="15"/>
+      <c r="BJ8" s="15"/>
+      <c r="BK8" s="15"/>
+      <c r="BL8" s="15"/>
+      <c r="BM8" s="24"/>
+      <c r="BN8" s="15"/>
+      <c r="BO8" s="15"/>
+      <c r="BP8" s="15"/>
+      <c r="BR8" s="24"/>
+    </row>
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" s="17"/>
+      <c r="E9" s="9"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
+      <c r="AN9" s="24"/>
+      <c r="AO9" s="15"/>
+      <c r="AP9" s="15"/>
+      <c r="AQ9" s="15"/>
+      <c r="AR9" s="15"/>
+      <c r="AS9" s="24"/>
+      <c r="AT9" s="15"/>
+      <c r="AU9" s="15"/>
+      <c r="AV9" s="15"/>
+      <c r="AW9" s="15"/>
+      <c r="AX9" s="24"/>
+      <c r="AY9" s="15"/>
+      <c r="AZ9" s="15"/>
+      <c r="BA9" s="15"/>
+      <c r="BB9" s="15"/>
+      <c r="BC9" s="24"/>
+      <c r="BD9" s="15"/>
+      <c r="BE9" s="15"/>
+      <c r="BF9" s="15"/>
+      <c r="BG9" s="15"/>
+      <c r="BH9" s="24"/>
+      <c r="BI9" s="15"/>
+      <c r="BJ9" s="15"/>
+      <c r="BK9" s="15"/>
+      <c r="BL9" s="15"/>
+      <c r="BM9" s="24"/>
+      <c r="BN9" s="15"/>
+      <c r="BO9" s="15"/>
+      <c r="BP9" s="15"/>
+      <c r="BR9" s="24"/>
+    </row>
+    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="18">
         <v>28</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="8">
+        <v>28</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" ref="H10:H15" si="5">IF(C10="Zoom",VALUE(RIGHT(D10,LEN(D10)-FIND("-",D10))),D10)</f>
+        <v>28</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
+      <c r="AN10" s="24"/>
+      <c r="AO10" s="15"/>
+      <c r="AP10" s="15"/>
+      <c r="AQ10" s="15"/>
+      <c r="AR10" s="15"/>
+      <c r="AS10" s="24"/>
+      <c r="AT10" s="15"/>
+      <c r="AU10" s="15"/>
+      <c r="AV10" s="15"/>
+      <c r="AW10" s="15"/>
+      <c r="AX10" s="24"/>
+      <c r="AY10" s="15"/>
+      <c r="AZ10" s="15"/>
+      <c r="BA10" s="15"/>
+      <c r="BB10" s="15"/>
+      <c r="BC10" s="24"/>
+      <c r="BD10" s="15"/>
+      <c r="BE10" s="15"/>
+      <c r="BF10" s="15"/>
+      <c r="BG10" s="15"/>
+      <c r="BH10" s="24"/>
+      <c r="BI10" s="15"/>
+      <c r="BJ10" s="15"/>
+      <c r="BK10" s="15"/>
+      <c r="BL10" s="15"/>
+      <c r="BM10" s="24"/>
+      <c r="BN10" s="15"/>
+      <c r="BO10" s="15"/>
+      <c r="BP10" s="15"/>
+      <c r="BR10" s="24"/>
+    </row>
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" s="8">
+        <v>28</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
+      <c r="AN11" s="24"/>
+      <c r="AO11" s="15"/>
+      <c r="AP11" s="15"/>
+      <c r="AQ11" s="15"/>
+      <c r="AR11" s="15"/>
+      <c r="AS11" s="24"/>
+      <c r="AT11" s="15"/>
+      <c r="AU11" s="15"/>
+      <c r="AV11" s="15"/>
+      <c r="AW11" s="15"/>
+      <c r="AX11" s="24"/>
+      <c r="AY11" s="15"/>
+      <c r="AZ11" s="15"/>
+      <c r="BA11" s="15"/>
+      <c r="BB11" s="15"/>
+      <c r="BC11" s="24"/>
+      <c r="BD11" s="15"/>
+      <c r="BE11" s="15"/>
+      <c r="BF11" s="15"/>
+      <c r="BG11" s="15"/>
+      <c r="BH11" s="24"/>
+      <c r="BI11" s="15"/>
+      <c r="BJ11" s="15"/>
+      <c r="BK11" s="15"/>
+      <c r="BL11" s="15"/>
+      <c r="BM11" s="24"/>
+      <c r="BN11" s="15"/>
+      <c r="BO11" s="15"/>
+      <c r="BP11" s="15"/>
+      <c r="BR11" s="24"/>
+    </row>
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="8">
+        <v>35</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="15"/>
+      <c r="AI12" s="15"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="15"/>
+      <c r="AL12" s="15"/>
+      <c r="AM12" s="15"/>
+      <c r="AN12" s="24"/>
+      <c r="AO12" s="15"/>
+      <c r="AP12" s="15"/>
+      <c r="AQ12" s="15"/>
+      <c r="AR12" s="15"/>
+      <c r="AS12" s="24"/>
+      <c r="AT12" s="15"/>
+      <c r="AU12" s="15"/>
+      <c r="AV12" s="15"/>
+      <c r="AW12" s="15"/>
+      <c r="AX12" s="24"/>
+      <c r="AY12" s="15"/>
+      <c r="AZ12" s="15"/>
+      <c r="BA12" s="15"/>
+      <c r="BB12" s="15"/>
+      <c r="BC12" s="24"/>
+      <c r="BD12" s="15"/>
+      <c r="BE12" s="15"/>
+      <c r="BF12" s="15"/>
+      <c r="BG12" s="15"/>
+      <c r="BH12" s="24"/>
+      <c r="BI12" s="15"/>
+      <c r="BJ12" s="15"/>
+      <c r="BK12" s="15"/>
+      <c r="BL12" s="15"/>
+      <c r="BM12" s="24"/>
+      <c r="BN12" s="15"/>
+      <c r="BO12" s="15"/>
+      <c r="BP12" s="15"/>
+      <c r="BR12" s="24"/>
+    </row>
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" s="8">
+        <v>35</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="24"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
+      <c r="AM13" s="15"/>
+      <c r="AN13" s="24"/>
+      <c r="AO13" s="15"/>
+      <c r="AP13" s="15"/>
+      <c r="AQ13" s="15"/>
+      <c r="AR13" s="15"/>
+      <c r="AS13" s="24"/>
+      <c r="AT13" s="15"/>
+      <c r="AU13" s="15"/>
+      <c r="AV13" s="15"/>
+      <c r="AW13" s="15"/>
+      <c r="AX13" s="24"/>
+      <c r="AY13" s="15"/>
+      <c r="AZ13" s="15"/>
+      <c r="BA13" s="15"/>
+      <c r="BB13" s="15"/>
+      <c r="BC13" s="24"/>
+      <c r="BD13" s="15"/>
+      <c r="BE13" s="15"/>
+      <c r="BF13" s="15"/>
+      <c r="BG13" s="15"/>
+      <c r="BH13" s="24"/>
+      <c r="BI13" s="15"/>
+      <c r="BJ13" s="15"/>
+      <c r="BK13" s="15"/>
+      <c r="BL13" s="15"/>
+      <c r="BM13" s="24"/>
+      <c r="BN13" s="15"/>
+      <c r="BO13" s="15"/>
+      <c r="BP13" s="15"/>
+      <c r="BR13" s="24"/>
+    </row>
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="18">
         <v>50</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" s="8">
+        <v>50</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+      <c r="AS14" s="24"/>
+      <c r="AT14" s="15"/>
+      <c r="AU14" s="15"/>
+      <c r="AV14" s="15"/>
+      <c r="AW14" s="15"/>
+      <c r="AX14" s="24"/>
+      <c r="AY14" s="15"/>
+      <c r="AZ14" s="15"/>
+      <c r="BA14" s="15"/>
+      <c r="BB14" s="15"/>
+      <c r="BC14" s="24"/>
+      <c r="BD14" s="15"/>
+      <c r="BE14" s="15"/>
+      <c r="BF14" s="15"/>
+      <c r="BG14" s="15"/>
+      <c r="BH14" s="24"/>
+      <c r="BI14" s="15"/>
+      <c r="BJ14" s="15"/>
+      <c r="BK14" s="15"/>
+      <c r="BL14" s="15"/>
+      <c r="BM14" s="24"/>
+      <c r="BN14" s="15"/>
+      <c r="BO14" s="15"/>
+      <c r="BP14" s="15"/>
+      <c r="BR14" s="24"/>
+    </row>
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-    </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" s="8">
+        <v>70</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+      <c r="AN15" s="24"/>
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="15"/>
+      <c r="AQ15" s="15"/>
+      <c r="AR15" s="15"/>
+      <c r="AS15" s="24"/>
+      <c r="AT15" s="15"/>
+      <c r="AU15" s="15"/>
+      <c r="AV15" s="15"/>
+      <c r="AW15" s="15"/>
+      <c r="AX15" s="24"/>
+      <c r="AY15" s="15"/>
+      <c r="AZ15" s="15"/>
+      <c r="BA15" s="15"/>
+      <c r="BB15" s="15"/>
+      <c r="BC15" s="24"/>
+      <c r="BD15" s="15"/>
+      <c r="BE15" s="15"/>
+      <c r="BF15" s="15"/>
+      <c r="BG15" s="15"/>
+      <c r="BH15" s="24"/>
+      <c r="BI15" s="15"/>
+      <c r="BJ15" s="15"/>
+      <c r="BK15" s="15"/>
+      <c r="BL15" s="15"/>
+      <c r="BM15" s="24"/>
+      <c r="BN15" s="15"/>
+      <c r="BO15" s="15"/>
+      <c r="BP15" s="15"/>
+      <c r="BR15" s="24"/>
+    </row>
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="I16" s="8"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="24"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="24"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="24"/>
+      <c r="AY16" s="15"/>
+      <c r="AZ16" s="15"/>
+      <c r="BA16" s="15"/>
+      <c r="BB16" s="15"/>
+      <c r="BC16" s="24"/>
+      <c r="BD16" s="15"/>
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="15"/>
+      <c r="BG16" s="15"/>
+      <c r="BH16" s="24"/>
+      <c r="BI16" s="15"/>
+      <c r="BJ16" s="15"/>
+      <c r="BK16" s="15"/>
+      <c r="BL16" s="15"/>
+      <c r="BM16" s="24"/>
+      <c r="BN16" s="15"/>
+      <c r="BO16" s="15"/>
+      <c r="BP16" s="15"/>
+      <c r="BR16" s="24"/>
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="15"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="24"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="24"/>
+      <c r="AT17" s="15"/>
+      <c r="AU17" s="15"/>
+      <c r="AV17" s="15"/>
+      <c r="AW17" s="15"/>
+      <c r="AX17" s="24"/>
+      <c r="AY17" s="15"/>
+      <c r="AZ17" s="15"/>
+      <c r="BA17" s="15"/>
+      <c r="BB17" s="15"/>
+      <c r="BC17" s="24"/>
+      <c r="BD17" s="15"/>
+      <c r="BE17" s="15"/>
+      <c r="BF17" s="15"/>
+      <c r="BG17" s="15"/>
+      <c r="BH17" s="24"/>
+      <c r="BI17" s="15"/>
+      <c r="BJ17" s="15"/>
+      <c r="BK17" s="15"/>
+      <c r="BL17" s="15"/>
+      <c r="BM17" s="24"/>
+      <c r="BN17" s="15"/>
+      <c r="BO17" s="15"/>
+      <c r="BP17" s="15"/>
+      <c r="BR17" s="24"/>
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="18">
         <v>28</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" s="8">
+        <v>28</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" ref="H18:H22" si="6">IF(C18="Zoom",VALUE(RIGHT(D18,LEN(D18)-FIND("-",D18))),D18)</f>
+        <v>28</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="15"/>
+      <c r="AL18" s="15"/>
+      <c r="AM18" s="15"/>
+      <c r="AN18" s="24"/>
+      <c r="AO18" s="15"/>
+      <c r="AP18" s="15"/>
+      <c r="AQ18" s="15"/>
+      <c r="AR18" s="15"/>
+      <c r="AS18" s="24"/>
+      <c r="AT18" s="15"/>
+      <c r="AU18" s="15"/>
+      <c r="AV18" s="15"/>
+      <c r="AW18" s="15"/>
+      <c r="AX18" s="24"/>
+      <c r="AY18" s="15"/>
+      <c r="AZ18" s="15"/>
+      <c r="BA18" s="15"/>
+      <c r="BB18" s="15"/>
+      <c r="BC18" s="24"/>
+      <c r="BD18" s="15"/>
+      <c r="BE18" s="15"/>
+      <c r="BF18" s="15"/>
+      <c r="BG18" s="15"/>
+      <c r="BH18" s="24"/>
+      <c r="BI18" s="15"/>
+      <c r="BJ18" s="15"/>
+      <c r="BK18" s="15"/>
+      <c r="BL18" s="15"/>
+      <c r="BM18" s="24"/>
+      <c r="BN18" s="15"/>
+      <c r="BO18" s="15"/>
+      <c r="BP18" s="15"/>
+      <c r="BR18" s="24"/>
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="18">
         <v>35</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19" s="8">
+        <v>35</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+      <c r="AN19" s="24"/>
+      <c r="AO19" s="15"/>
+      <c r="AP19" s="15"/>
+      <c r="AQ19" s="15"/>
+      <c r="AR19" s="15"/>
+      <c r="AS19" s="24"/>
+      <c r="AT19" s="15"/>
+      <c r="AU19" s="15"/>
+      <c r="AV19" s="15"/>
+      <c r="AW19" s="15"/>
+      <c r="AX19" s="24"/>
+      <c r="AY19" s="15"/>
+      <c r="AZ19" s="15"/>
+      <c r="BA19" s="15"/>
+      <c r="BB19" s="15"/>
+      <c r="BC19" s="24"/>
+      <c r="BD19" s="15"/>
+      <c r="BE19" s="15"/>
+      <c r="BF19" s="15"/>
+      <c r="BG19" s="15"/>
+      <c r="BH19" s="24"/>
+      <c r="BI19" s="15"/>
+      <c r="BJ19" s="15"/>
+      <c r="BK19" s="15"/>
+      <c r="BL19" s="15"/>
+      <c r="BM19" s="24"/>
+      <c r="BN19" s="15"/>
+      <c r="BO19" s="15"/>
+      <c r="BP19" s="15"/>
+      <c r="BR19" s="24"/>
+    </row>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="18">
         <v>50</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="BD20" s="5"/>
-    </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" s="8">
+        <v>50</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+      <c r="AN20" s="24"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="24"/>
+      <c r="AT20" s="15"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+      <c r="AW20" s="15"/>
+      <c r="AX20" s="24"/>
+      <c r="AY20" s="15"/>
+      <c r="AZ20" s="15"/>
+      <c r="BA20" s="15"/>
+      <c r="BB20" s="15"/>
+      <c r="BC20" s="24"/>
+      <c r="BD20" s="15"/>
+      <c r="BE20" s="15"/>
+      <c r="BF20" s="15"/>
+      <c r="BG20" s="15"/>
+      <c r="BH20" s="24"/>
+      <c r="BI20" s="15"/>
+      <c r="BJ20" s="15"/>
+      <c r="BK20" s="15"/>
+      <c r="BL20" s="15"/>
+      <c r="BM20" s="24"/>
+      <c r="BN20" s="15"/>
+      <c r="BO20" s="15"/>
+      <c r="BP20" s="15"/>
+      <c r="BR20" s="24"/>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="18">
         <v>135</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="S21" s="18"/>
-      <c r="BD21" s="5"/>
-    </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" s="8">
+        <v>135</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="6"/>
+        <v>135</v>
+      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="24"/>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="15"/>
+      <c r="AH21" s="15"/>
+      <c r="AI21" s="15"/>
+      <c r="AJ21" s="15"/>
+      <c r="AK21" s="15"/>
+      <c r="AL21" s="15"/>
+      <c r="AM21" s="15"/>
+      <c r="AN21" s="24"/>
+      <c r="AO21" s="15"/>
+      <c r="AP21" s="15"/>
+      <c r="AQ21" s="15"/>
+      <c r="AR21" s="15"/>
+      <c r="AS21" s="24"/>
+      <c r="AT21" s="15"/>
+      <c r="AU21" s="15"/>
+      <c r="AV21" s="15"/>
+      <c r="AW21" s="15"/>
+      <c r="AX21" s="24"/>
+      <c r="AY21" s="15"/>
+      <c r="AZ21" s="15"/>
+      <c r="BA21" s="15"/>
+      <c r="BB21" s="15"/>
+      <c r="BC21" s="24"/>
+      <c r="BD21" s="15"/>
+      <c r="BE21" s="15"/>
+      <c r="BF21" s="15"/>
+      <c r="BG21" s="15"/>
+      <c r="BH21" s="24"/>
+      <c r="BI21" s="15"/>
+      <c r="BJ21" s="15"/>
+      <c r="BK21" s="15"/>
+      <c r="BL21" s="15"/>
+      <c r="BM21" s="24"/>
+      <c r="BN21" s="15"/>
+      <c r="BO21" s="15"/>
+      <c r="BP21" s="15"/>
+      <c r="BR21" s="24"/>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="18">
         <v>500</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="BD22" s="4"/>
-    </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.55000000000000004">
-      <c r="D23" s="11"/>
-      <c r="BD23" s="5"/>
-    </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G22" s="8">
+        <v>500</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="24"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="15"/>
+      <c r="AL22" s="15"/>
+      <c r="AM22" s="15"/>
+      <c r="AN22" s="24"/>
+      <c r="AO22" s="15"/>
+      <c r="AP22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+      <c r="AS22" s="24"/>
+      <c r="AT22" s="15"/>
+      <c r="AU22" s="15"/>
+      <c r="AV22" s="15"/>
+      <c r="AW22" s="15"/>
+      <c r="AX22" s="24"/>
+      <c r="AY22" s="15"/>
+      <c r="AZ22" s="15"/>
+      <c r="BA22" s="15"/>
+      <c r="BB22" s="15"/>
+      <c r="BC22" s="24"/>
+      <c r="BD22" s="15"/>
+      <c r="BE22" s="15"/>
+      <c r="BF22" s="15"/>
+      <c r="BG22" s="15"/>
+      <c r="BH22" s="24"/>
+      <c r="BI22" s="15"/>
+      <c r="BJ22" s="15"/>
+      <c r="BK22" s="15"/>
+      <c r="BL22" s="15"/>
+      <c r="BM22" s="24"/>
+      <c r="BN22" s="15"/>
+      <c r="BO22" s="15"/>
+      <c r="BP22" s="15"/>
+      <c r="BR22" s="24"/>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="E23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="24"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="15"/>
+      <c r="AJ23" s="15"/>
+      <c r="AK23" s="15"/>
+      <c r="AL23" s="15"/>
+      <c r="AM23" s="15"/>
+      <c r="AN23" s="24"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+      <c r="AR23" s="15"/>
+      <c r="AS23" s="24"/>
+      <c r="AT23" s="15"/>
+      <c r="AU23" s="15"/>
+      <c r="AV23" s="15"/>
+      <c r="AW23" s="15"/>
+      <c r="AX23" s="24"/>
+      <c r="AY23" s="15"/>
+      <c r="AZ23" s="15"/>
+      <c r="BA23" s="15"/>
+      <c r="BB23" s="15"/>
+      <c r="BC23" s="24"/>
+      <c r="BD23" s="15"/>
+      <c r="BE23" s="15"/>
+      <c r="BF23" s="15"/>
+      <c r="BG23" s="15"/>
+      <c r="BH23" s="24"/>
+      <c r="BI23" s="15"/>
+      <c r="BJ23" s="15"/>
+      <c r="BK23" s="15"/>
+      <c r="BL23" s="15"/>
+      <c r="BM23" s="24"/>
+      <c r="BN23" s="15"/>
+      <c r="BO23" s="15"/>
+      <c r="BP23" s="15"/>
+      <c r="BR23" s="24"/>
+    </row>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="BD24" s="5"/>
-    </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="24"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="24"/>
+      <c r="AT24" s="15"/>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="15"/>
+      <c r="AW24" s="15"/>
+      <c r="AX24" s="24"/>
+      <c r="AY24" s="15"/>
+      <c r="AZ24" s="15"/>
+      <c r="BA24" s="15"/>
+      <c r="BB24" s="15"/>
+      <c r="BC24" s="24"/>
+      <c r="BD24" s="15"/>
+      <c r="BE24" s="15"/>
+      <c r="BF24" s="15"/>
+      <c r="BG24" s="15"/>
+      <c r="BH24" s="24"/>
+      <c r="BI24" s="15"/>
+      <c r="BJ24" s="15"/>
+      <c r="BK24" s="15"/>
+      <c r="BL24" s="15"/>
+      <c r="BM24" s="24"/>
+      <c r="BN24" s="15"/>
+      <c r="BO24" s="15"/>
+      <c r="BP24" s="15"/>
+      <c r="BR24" s="24"/>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="18">
         <v>85</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="N25" s="18"/>
-      <c r="BD25" s="5"/>
-    </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25" s="8">
+        <v>85</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" ref="H25:H26" si="7">IF(C25="Zoom",VALUE(RIGHT(D25,LEN(D25)-FIND("-",D25))),D25)</f>
+        <v>85</v>
+      </c>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="15"/>
+      <c r="AH25" s="15"/>
+      <c r="AI25" s="15"/>
+      <c r="AJ25" s="15"/>
+      <c r="AK25" s="15"/>
+      <c r="AL25" s="15"/>
+      <c r="AM25" s="15"/>
+      <c r="AN25" s="24"/>
+      <c r="AO25" s="15"/>
+      <c r="AP25" s="15"/>
+      <c r="AQ25" s="15"/>
+      <c r="AR25" s="15"/>
+      <c r="AS25" s="24"/>
+      <c r="AT25" s="15"/>
+      <c r="AU25" s="15"/>
+      <c r="AV25" s="15"/>
+      <c r="AW25" s="15"/>
+      <c r="AX25" s="24"/>
+      <c r="AY25" s="15"/>
+      <c r="AZ25" s="15"/>
+      <c r="BA25" s="15"/>
+      <c r="BB25" s="15"/>
+      <c r="BC25" s="24"/>
+      <c r="BD25" s="15"/>
+      <c r="BE25" s="15"/>
+      <c r="BF25" s="15"/>
+      <c r="BG25" s="15"/>
+      <c r="BH25" s="24"/>
+      <c r="BI25" s="15"/>
+      <c r="BJ25" s="15"/>
+      <c r="BK25" s="15"/>
+      <c r="BL25" s="15"/>
+      <c r="BM25" s="24"/>
+      <c r="BN25" s="15"/>
+      <c r="BO25" s="15"/>
+      <c r="BP25" s="15"/>
+      <c r="BR25" s="24"/>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="18">
         <v>55</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K26" s="18"/>
-    </row>
-    <row r="27" spans="1:66" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="8" t="s">
+      <c r="G26" s="8">
+        <v>55</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="7"/>
+        <v>55</v>
+      </c>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="15"/>
+      <c r="AI26" s="15"/>
+      <c r="AJ26" s="15"/>
+      <c r="AK26" s="15"/>
+      <c r="AL26" s="15"/>
+      <c r="AM26" s="15"/>
+      <c r="AN26" s="24"/>
+      <c r="AO26" s="15"/>
+      <c r="AP26" s="15"/>
+      <c r="AQ26" s="15"/>
+      <c r="AR26" s="15"/>
+      <c r="AS26" s="24"/>
+      <c r="AT26" s="15"/>
+      <c r="AU26" s="15"/>
+      <c r="AV26" s="15"/>
+      <c r="AW26" s="15"/>
+      <c r="AX26" s="24"/>
+      <c r="AY26" s="15"/>
+      <c r="AZ26" s="15"/>
+      <c r="BA26" s="15"/>
+      <c r="BB26" s="15"/>
+      <c r="BC26" s="24"/>
+      <c r="BD26" s="15"/>
+      <c r="BE26" s="15"/>
+      <c r="BF26" s="15"/>
+      <c r="BG26" s="15"/>
+      <c r="BH26" s="24"/>
+      <c r="BI26" s="15"/>
+      <c r="BJ26" s="15"/>
+      <c r="BK26" s="15"/>
+      <c r="BL26" s="15"/>
+      <c r="BM26" s="24"/>
+      <c r="BN26" s="15"/>
+      <c r="BO26" s="15"/>
+      <c r="BP26" s="15"/>
+      <c r="BR26" s="24"/>
+    </row>
+    <row r="27" spans="1:70" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="7">
+      <c r="D27" s="19"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="21">
         <v>0</v>
       </c>
-      <c r="G27" s="7">
-        <f>F27+10</f>
+      <c r="J27" s="21">
         <v>10</v>
       </c>
-      <c r="H27" s="7">
-        <f t="shared" ref="H27:BN27" si="0">G27+10</f>
+      <c r="K27" s="21">
+        <f>J27+2</f>
+        <v>12</v>
+      </c>
+      <c r="L27" s="21">
+        <f t="shared" ref="L27:Q27" si="8">K27+2</f>
+        <v>14</v>
+      </c>
+      <c r="M27" s="21">
+        <v>15</v>
+      </c>
+      <c r="N27" s="21">
+        <v>18</v>
+      </c>
+      <c r="O27" s="21">
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="I27" s="7">
-        <f t="shared" si="0"/>
+      <c r="P27" s="21">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Q27" s="22">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="R27" s="21">
+        <f>Q27+4</f>
+        <v>28</v>
+      </c>
+      <c r="S27" s="21">
         <v>30</v>
       </c>
-      <c r="J27" s="7">
-        <f t="shared" si="0"/>
+      <c r="T27" s="21">
+        <f t="shared" ref="T27:Y27" si="9">S27+5</f>
+        <v>35</v>
+      </c>
+      <c r="U27" s="21">
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="K27" s="7">
-        <f t="shared" si="0"/>
+      <c r="V27" s="21">
+        <v>43</v>
+      </c>
+      <c r="W27" s="22">
         <v>50</v>
       </c>
-      <c r="L27" s="7">
-        <f t="shared" si="0"/>
+      <c r="X27" s="21">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="Y27" s="21">
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="M27" s="7">
-        <f t="shared" si="0"/>
+      <c r="Z27" s="21">
         <v>70</v>
       </c>
-      <c r="N27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AA27" s="21">
+        <v>77</v>
+      </c>
+      <c r="AB27" s="21">
         <v>80</v>
       </c>
-      <c r="O27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AC27" s="21">
+        <v>85</v>
+      </c>
+      <c r="AD27" s="21">
+        <f>AB27+10</f>
         <v>90</v>
       </c>
-      <c r="P27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AE27" s="22">
+        <f t="shared" ref="AE27:AM27" si="10">AD27+10</f>
         <v>100</v>
       </c>
-      <c r="Q27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AF27" s="21">
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
-      <c r="R27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AG27" s="21">
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="S27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AH27" s="21">
+        <f t="shared" si="10"/>
         <v>130</v>
       </c>
-      <c r="T27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AI27" s="21">
+        <f t="shared" si="10"/>
         <v>140</v>
       </c>
-      <c r="U27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AJ27" s="21">
+        <f t="shared" si="10"/>
         <v>150</v>
       </c>
-      <c r="V27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AK27" s="21">
+        <f t="shared" si="10"/>
         <v>160</v>
       </c>
-      <c r="W27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AL27" s="21">
+        <f t="shared" si="10"/>
         <v>170</v>
       </c>
-      <c r="X27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AM27" s="21">
+        <f t="shared" si="10"/>
         <v>180</v>
       </c>
-      <c r="Y27" s="7">
-        <f t="shared" si="0"/>
-        <v>190</v>
-      </c>
-      <c r="Z27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AN27" s="22">
+        <f>AM27+20</f>
         <v>200</v>
       </c>
-      <c r="AA27" s="7">
-        <f t="shared" si="0"/>
-        <v>210</v>
-      </c>
-      <c r="AB27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AO27" s="21">
+        <f t="shared" ref="AO27:BR27" si="11">AN27+20</f>
         <v>220</v>
       </c>
-      <c r="AC27" s="7">
-        <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-      <c r="AD27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AP27" s="21">
+        <f t="shared" si="11"/>
         <v>240</v>
       </c>
-      <c r="AE27" s="7">
-        <f>AD27+10</f>
-        <v>250</v>
-      </c>
-      <c r="AF27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AQ27" s="21">
+        <f t="shared" si="11"/>
         <v>260</v>
       </c>
-      <c r="AG27" s="7">
-        <f t="shared" si="0"/>
-        <v>270</v>
-      </c>
-      <c r="AH27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AR27" s="21">
+        <f t="shared" si="11"/>
         <v>280</v>
       </c>
-      <c r="AI27" s="7">
-        <f t="shared" si="0"/>
-        <v>290</v>
-      </c>
-      <c r="AJ27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AS27" s="22">
+        <f t="shared" si="11"/>
         <v>300</v>
       </c>
-      <c r="AK27" s="7">
-        <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="AL27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AT27" s="21">
+        <f t="shared" si="11"/>
         <v>320</v>
       </c>
-      <c r="AM27" s="7">
-        <f t="shared" si="0"/>
-        <v>330</v>
-      </c>
-      <c r="AN27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AU27" s="21">
+        <f t="shared" si="11"/>
         <v>340</v>
       </c>
-      <c r="AO27" s="7">
-        <f t="shared" si="0"/>
-        <v>350</v>
-      </c>
-      <c r="AP27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AV27" s="21">
+        <f t="shared" si="11"/>
         <v>360</v>
       </c>
-      <c r="AQ27" s="7">
-        <f t="shared" si="0"/>
-        <v>370</v>
-      </c>
-      <c r="AR27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AW27" s="21">
+        <f t="shared" si="11"/>
         <v>380</v>
       </c>
-      <c r="AS27" s="7">
-        <f t="shared" si="0"/>
-        <v>390</v>
-      </c>
-      <c r="AT27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AX27" s="22">
+        <f t="shared" si="11"/>
         <v>400</v>
       </c>
-      <c r="AU27" s="7">
-        <f t="shared" si="0"/>
-        <v>410</v>
-      </c>
-      <c r="AV27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AY27" s="21">
+        <f t="shared" si="11"/>
         <v>420</v>
       </c>
-      <c r="AW27" s="7">
-        <f t="shared" si="0"/>
-        <v>430</v>
-      </c>
-      <c r="AX27" s="7">
-        <f t="shared" si="0"/>
+      <c r="AZ27" s="21">
+        <f t="shared" si="11"/>
         <v>440</v>
       </c>
-      <c r="AY27" s="7">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="AZ27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BA27" s="21">
+        <f t="shared" si="11"/>
         <v>460</v>
       </c>
-      <c r="BA27" s="7">
-        <f t="shared" si="0"/>
-        <v>470</v>
-      </c>
-      <c r="BB27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BB27" s="21">
+        <f t="shared" si="11"/>
         <v>480</v>
       </c>
-      <c r="BC27" s="7">
-        <f>BB27+10</f>
-        <v>490</v>
-      </c>
-      <c r="BD27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BC27" s="22">
+        <f t="shared" si="11"/>
         <v>500</v>
       </c>
-      <c r="BE27" s="7">
-        <f t="shared" si="0"/>
-        <v>510</v>
-      </c>
-      <c r="BF27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BD27" s="21">
+        <f>BC27+20</f>
         <v>520</v>
       </c>
-      <c r="BG27" s="7">
-        <f t="shared" si="0"/>
-        <v>530</v>
-      </c>
-      <c r="BH27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BE27" s="21">
+        <f t="shared" si="11"/>
         <v>540</v>
       </c>
-      <c r="BI27" s="7">
-        <f t="shared" si="0"/>
-        <v>550</v>
-      </c>
-      <c r="BJ27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BF27" s="21">
+        <f t="shared" si="11"/>
         <v>560</v>
       </c>
-      <c r="BK27" s="7">
-        <f t="shared" si="0"/>
-        <v>570</v>
-      </c>
-      <c r="BL27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BG27" s="21">
+        <f t="shared" si="11"/>
         <v>580</v>
       </c>
-      <c r="BM27" s="7">
-        <f t="shared" si="0"/>
-        <v>590</v>
-      </c>
-      <c r="BN27" s="7">
-        <f t="shared" si="0"/>
+      <c r="BH27" s="22">
+        <f t="shared" si="11"/>
         <v>600</v>
       </c>
-    </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+      <c r="BI27" s="21">
+        <f>BH27+20</f>
+        <v>620</v>
+      </c>
+      <c r="BJ27" s="21">
+        <f t="shared" si="11"/>
+        <v>640</v>
+      </c>
+      <c r="BK27" s="21">
+        <f t="shared" si="11"/>
+        <v>660</v>
+      </c>
+      <c r="BL27" s="21">
+        <f t="shared" si="11"/>
+        <v>680</v>
+      </c>
+      <c r="BM27" s="22">
+        <f t="shared" si="11"/>
+        <v>700</v>
+      </c>
+      <c r="BN27" s="21">
+        <f t="shared" si="11"/>
+        <v>720</v>
+      </c>
+      <c r="BO27" s="21">
+        <f t="shared" si="11"/>
+        <v>740</v>
+      </c>
+      <c r="BP27" s="21">
+        <f t="shared" si="11"/>
+        <v>760</v>
+      </c>
+      <c r="BQ27" s="21">
+        <f t="shared" si="11"/>
+        <v>780</v>
+      </c>
+      <c r="BR27" s="22">
+        <f t="shared" si="11"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:BN1"/>
+    <mergeCell ref="I1:BR1"/>
   </mergeCells>
+  <conditionalFormatting sqref="I25:P26 J23:P24 I18:P22 J16:P17 I10:P15 J8:P9 I3:P7 Q3:BR26">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND($G3&lt;=I$2,$H3&gt;=I$2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>